<commit_message>
edit dikit untuk presentasi
</commit_message>
<xml_diff>
--- a/backend/web/write.xlsx
+++ b/backend/web/write.xlsx
@@ -56,7 +56,7 @@
     <t>Kelas</t>
   </si>
   <si>
-    <t>A</t>
+    <t>B</t>
   </si>
   <si>
     <t>Pengampu</t>
@@ -634,7 +634,7 @@
         <v>5</v>
       </c>
       <c r="C6" s="10">
-        <v>2019</v>
+        <v>2014</v>
       </c>
       <c r="D6" s="10"/>
       <c r="E6" s="10"/>

</xml_diff>